<commit_message>
Updated MR dates and counting projects w MR
</commit_message>
<xml_diff>
--- a/G Knitting Projects 2004-2024.xlsx
+++ b/G Knitting Projects 2004-2024.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="638">
   <si>
     <t>Started</t>
   </si>
@@ -4740,15 +4740,24 @@
     <t>Retrograde Sign Element</t>
   </si>
   <si>
+    <t>aries</t>
+  </si>
+  <si>
+    <t>Fire</t>
+  </si>
+  <si>
+    <t>Virgo</t>
+  </si>
+  <si>
+    <t>Earth</t>
+  </si>
+  <si>
+    <t>Sagittarius</t>
+  </si>
+  <si>
     <t>Taurus</t>
   </si>
   <si>
-    <t>Earth</t>
-  </si>
-  <si>
-    <t>Virgo</t>
-  </si>
-  <si>
     <t>Capricorn</t>
   </si>
   <si>
@@ -4779,26 +4788,43 @@
     <t>Leo</t>
   </si>
   <si>
-    <t>Fire</t>
-  </si>
-  <si>
     <t>Aries</t>
   </si>
   <si>
-    <t>Sagittarius</t>
+    <t>libra</t>
+  </si>
+  <si>
+    <t>pisces</t>
+  </si>
+  <si>
+    <t>scorpio</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>leo</t>
+  </si>
+  <si>
+    <t>sagittarius</t>
+  </si>
+  <si>
+    <t>capricorn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="4">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
     <numFmt numFmtId="165" formatCode="mmm d"/>
     <numFmt numFmtId="166" formatCode="mmmm d"/>
     <numFmt numFmtId="167" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="168" formatCode="mmm d, yyyy"/>
+    <numFmt numFmtId="169" formatCode="mmmm d, yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -4830,13 +4856,31 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <color rgb="FF414141"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -4845,7 +4889,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -4878,6 +4922,24 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="168" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="169" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="168" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -13487,6 +13549,12 @@
       <c r="C2" s="10">
         <v>45406.0</v>
       </c>
+      <c r="D2" s="9" t="s">
+        <v>614</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>615</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="9">
@@ -13498,6 +13566,12 @@
       <c r="C3" s="10">
         <v>45531.0</v>
       </c>
+      <c r="D3" s="9" t="s">
+        <v>616</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>617</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="9">
@@ -13509,6 +13583,12 @@
       <c r="C4" s="10">
         <v>45641.0</v>
       </c>
+      <c r="D4" s="9" t="s">
+        <v>618</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>615</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="9">
@@ -13521,10 +13601,10 @@
         <v>45060.0</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>614</v>
+        <v>619</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
     </row>
     <row r="6">
@@ -13541,7 +13621,7 @@
         <v>616</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
     </row>
     <row r="7">
@@ -13555,10 +13635,10 @@
         <v>45292.0</v>
       </c>
       <c r="D7" s="9" t="s">
+        <v>620</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>617</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="8">
@@ -13572,10 +13652,10 @@
         <v>44944.0</v>
       </c>
       <c r="D8" s="9" t="s">
+        <v>620</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>617</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="9">
@@ -13589,10 +13669,10 @@
         <v>44595.0</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
     </row>
     <row r="10">
@@ -13606,10 +13686,10 @@
         <v>44715.0</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
     </row>
     <row r="11">
@@ -13623,10 +13703,10 @@
         <v>44836.0</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
     </row>
     <row r="12">
@@ -13640,10 +13720,10 @@
         <v>44247.0</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
     </row>
     <row r="13">
@@ -13657,10 +13737,10 @@
         <v>44369.0</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
     </row>
     <row r="14">
@@ -13674,10 +13754,10 @@
         <v>44487.0</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
     </row>
     <row r="15">
@@ -13691,10 +13771,10 @@
         <v>43899.0</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
     </row>
     <row r="16">
@@ -13708,10 +13788,10 @@
         <v>44024.0</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
     </row>
     <row r="17">
@@ -13725,10 +13805,10 @@
         <v>44138.0</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
     </row>
     <row r="18">
@@ -13742,10 +13822,10 @@
         <v>43552.0</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
     </row>
     <row r="19">
@@ -13759,10 +13839,10 @@
         <v>43677.0</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>627</v>
+        <v>615</v>
       </c>
     </row>
     <row r="20">
@@ -13776,10 +13856,10 @@
         <v>43789.0</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
     </row>
     <row r="21">
@@ -13793,10 +13873,10 @@
         <v>43205.0</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>627</v>
+        <v>615</v>
       </c>
     </row>
     <row r="22">
@@ -13810,10 +13890,10 @@
         <v>43330.0</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>627</v>
+        <v>615</v>
       </c>
     </row>
     <row r="23">
@@ -13827,10 +13907,10 @@
         <v>43440.0</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>629</v>
+        <v>618</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>627</v>
+        <v>615</v>
       </c>
     </row>
     <row r="24">
@@ -13844,10 +13924,10 @@
         <v>42858.0</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>614</v>
+        <v>619</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
     </row>
     <row r="25">
@@ -13864,7 +13944,7 @@
         <v>616</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
     </row>
     <row r="26">
@@ -13878,10 +13958,10 @@
         <v>43091.0</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>629</v>
+        <v>618</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>627</v>
+        <v>615</v>
       </c>
     </row>
     <row r="27">
@@ -13895,10 +13975,10 @@
         <v>42743.0</v>
       </c>
       <c r="D27" s="9" t="s">
+        <v>620</v>
+      </c>
+      <c r="E27" s="9" t="s">
         <v>617</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="28">
@@ -13912,10 +13992,10 @@
         <v>42394.0</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
     </row>
     <row r="29">
@@ -13929,10 +14009,10 @@
         <v>42512.0</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>614</v>
+        <v>619</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
     </row>
     <row r="30">
@@ -13949,12 +14029,670 @@
         <v>616</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="9">
         <v>2015.0</v>
+      </c>
+      <c r="B31" s="13">
+        <v>42025.0</v>
+      </c>
+      <c r="C31" s="13">
+        <v>42046.0</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>621</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="9">
+        <v>2015.0</v>
+      </c>
+      <c r="B32" s="14">
+        <v>42143.0</v>
+      </c>
+      <c r="C32" s="13">
+        <v>42166.0</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>623</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="9">
+        <v>2015.0</v>
+      </c>
+      <c r="B33" s="13">
+        <v>42264.0</v>
+      </c>
+      <c r="C33" s="15">
+        <v>42286.0</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>624</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="9">
+        <v>2014.0</v>
+      </c>
+      <c r="B34" s="13">
+        <v>41676.0</v>
+      </c>
+      <c r="C34" s="13">
+        <v>41698.0</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>625</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="9">
+        <v>2014.0</v>
+      </c>
+      <c r="B35" s="13">
+        <v>41797.0</v>
+      </c>
+      <c r="C35" s="13">
+        <v>41821.0</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>627</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="9">
+        <v>2014.0</v>
+      </c>
+      <c r="B36" s="13">
+        <v>41916.0</v>
+      </c>
+      <c r="C36" s="15">
+        <v>41937.0</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>628</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="9">
+        <v>2013.0</v>
+      </c>
+      <c r="B37" s="13">
+        <v>41328.0</v>
+      </c>
+      <c r="C37" s="13">
+        <v>41350.0</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>625</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="9">
+        <v>2013.0</v>
+      </c>
+      <c r="B38" s="13">
+        <v>41451.0</v>
+      </c>
+      <c r="C38" s="13">
+        <v>41475.0</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>627</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="9">
+        <v>2013.0</v>
+      </c>
+      <c r="B39" s="13">
+        <v>41568.0</v>
+      </c>
+      <c r="C39" s="15">
+        <v>41588.0</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>628</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="9">
+        <v>2012.0</v>
+      </c>
+      <c r="B40" s="13">
+        <v>40980.0</v>
+      </c>
+      <c r="C40" s="13">
+        <v>41003.0</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>630</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="9">
+        <v>2012.0</v>
+      </c>
+      <c r="B41" s="13">
+        <v>41105.0</v>
+      </c>
+      <c r="C41" s="13">
+        <v>41129.0</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>629</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="9">
+        <v>2012.0</v>
+      </c>
+      <c r="B42" s="13">
+        <v>41219.0</v>
+      </c>
+      <c r="C42" s="15">
+        <v>41239.0</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>618</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="9">
+        <v>2011.0</v>
+      </c>
+      <c r="B43" s="13">
+        <v>40632.0</v>
+      </c>
+      <c r="C43" s="13">
+        <v>40656.0</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>630</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="9">
+        <v>2011.0</v>
+      </c>
+      <c r="B44" s="13">
+        <v>40758.0</v>
+      </c>
+      <c r="C44" s="13">
+        <v>40781.0</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>616</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="9">
+        <v>2011.0</v>
+      </c>
+      <c r="B45" s="13">
+        <v>40871.0</v>
+      </c>
+      <c r="C45" s="15">
+        <v>40891.0</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>618</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="9">
+        <v>2010.0</v>
+      </c>
+      <c r="B46" s="13">
+        <v>40173.0</v>
+      </c>
+      <c r="C46" s="13">
+        <v>40193.0</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>620</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="9">
+        <v>2010.0</v>
+      </c>
+      <c r="B47" s="13">
+        <v>40286.0</v>
+      </c>
+      <c r="C47" s="14">
+        <v>40309.0</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>619</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="9">
+        <v>2010.0</v>
+      </c>
+      <c r="B48" s="13">
+        <v>40410.0</v>
+      </c>
+      <c r="C48" s="13">
+        <v>40433.0</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>616</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="9">
+        <v>2010.0</v>
+      </c>
+      <c r="B49" s="13">
+        <v>40522.0</v>
+      </c>
+      <c r="C49" s="15">
+        <v>40542.0</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>620</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="9">
+        <v>2009.0</v>
+      </c>
+      <c r="B50" s="13">
+        <v>39824.0</v>
+      </c>
+      <c r="C50" s="13">
+        <v>39845.0</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E50" s="17" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="9">
+        <v>2009.0</v>
+      </c>
+      <c r="B51" s="14">
+        <v>39940.0</v>
+      </c>
+      <c r="C51" s="14">
+        <v>39964.0</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>623</v>
+      </c>
+      <c r="E51" s="17" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="9">
+        <v>2009.0</v>
+      </c>
+      <c r="B52" s="13">
+        <v>40063.0</v>
+      </c>
+      <c r="C52" s="13">
+        <v>40085.0</v>
+      </c>
+      <c r="D52" s="16" t="s">
+        <v>624</v>
+      </c>
+      <c r="E52" s="17" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="9">
+        <v>2009.0</v>
+      </c>
+      <c r="B53" s="13">
+        <v>40173.0</v>
+      </c>
+      <c r="C53" s="15">
+        <v>40193.0</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>620</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="9">
+        <v>2008.0</v>
+      </c>
+      <c r="B54" s="13">
+        <v>39475.0</v>
+      </c>
+      <c r="C54" s="13">
+        <v>39497.0</v>
+      </c>
+      <c r="D54" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="E54" s="17" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="9">
+        <v>2008.0</v>
+      </c>
+      <c r="B55" s="14">
+        <v>39594.0</v>
+      </c>
+      <c r="C55" s="13">
+        <v>39618.0</v>
+      </c>
+      <c r="D55" s="16" t="s">
+        <v>623</v>
+      </c>
+      <c r="E55" s="17" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="9">
+        <v>2008.0</v>
+      </c>
+      <c r="B56" s="13">
+        <v>39715.0</v>
+      </c>
+      <c r="C56" s="15">
+        <v>39736.0</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>631</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="9">
+        <v>2007.0</v>
+      </c>
+      <c r="B57" s="12">
+        <v>39127.0</v>
+      </c>
+      <c r="C57" s="12">
+        <v>39149.0</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>632</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="9">
+        <v>2007.0</v>
+      </c>
+      <c r="B58" s="18">
+        <v>39248.0</v>
+      </c>
+      <c r="C58" s="18">
+        <v>39273.0</v>
+      </c>
+      <c r="D58" s="16" t="s">
+        <v>627</v>
+      </c>
+      <c r="E58" s="17" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="9">
+        <v>2007.0</v>
+      </c>
+      <c r="B59" s="18">
+        <v>39367.0</v>
+      </c>
+      <c r="C59" s="15">
+        <v>39387.0</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>633</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="9">
+        <v>2006.0</v>
+      </c>
+      <c r="B60" s="13">
+        <v>38778.0</v>
+      </c>
+      <c r="C60" s="13">
+        <v>38801.0</v>
+      </c>
+      <c r="D60" s="16" t="s">
+        <v>632</v>
+      </c>
+      <c r="E60" s="17" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="9">
+        <v>2006.0</v>
+      </c>
+      <c r="B61" s="13">
+        <v>38902.0</v>
+      </c>
+      <c r="C61" s="13">
+        <v>38927.0</v>
+      </c>
+      <c r="D61" s="16" t="s">
+        <v>629</v>
+      </c>
+      <c r="E61" s="17" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="9">
+        <v>2006.0</v>
+      </c>
+      <c r="B62" s="13">
+        <v>39018.0</v>
+      </c>
+      <c r="C62" s="15">
+        <v>39039.0</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>633</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="9">
+        <v>2005.0</v>
+      </c>
+      <c r="B63" s="13">
+        <v>38431.0</v>
+      </c>
+      <c r="C63" s="13">
+        <v>38454.0</v>
+      </c>
+      <c r="D63" s="16" t="s">
+        <v>614</v>
+      </c>
+      <c r="E63" s="17" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="9">
+        <v>2005.0</v>
+      </c>
+      <c r="B64" s="13">
+        <v>38556.0</v>
+      </c>
+      <c r="C64" s="13">
+        <v>38580.0</v>
+      </c>
+      <c r="D64" s="16" t="s">
+        <v>635</v>
+      </c>
+      <c r="E64" s="17" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="9">
+        <v>2005.0</v>
+      </c>
+      <c r="B65" s="13">
+        <v>38670.0</v>
+      </c>
+      <c r="C65" s="15">
+        <v>38690.0</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>636</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="9">
+        <v>2004.0</v>
+      </c>
+      <c r="B66" s="13">
+        <v>37972.0</v>
+      </c>
+      <c r="C66" s="13">
+        <v>37992.0</v>
+      </c>
+      <c r="D66" s="16" t="s">
+        <v>637</v>
+      </c>
+      <c r="E66" s="17" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="9">
+        <v>2004.0</v>
+      </c>
+      <c r="B67" s="13">
+        <v>38083.0</v>
+      </c>
+      <c r="C67" s="13">
+        <v>38107.0</v>
+      </c>
+      <c r="D67" s="16" t="s">
+        <v>619</v>
+      </c>
+      <c r="E67" s="17" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="9">
+        <v>2004.0</v>
+      </c>
+      <c r="B68" s="13">
+        <v>38209.0</v>
+      </c>
+      <c r="C68" s="13">
+        <v>38232.0</v>
+      </c>
+      <c r="D68" s="16" t="s">
+        <v>616</v>
+      </c>
+      <c r="E68" s="17" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="9">
+        <v>2004.0</v>
+      </c>
+      <c r="B69" s="13">
+        <v>38321.0</v>
+      </c>
+      <c r="C69" s="15">
+        <v>38341.0</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>636</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>615</v>
       </c>
     </row>
   </sheetData>

</xml_diff>